<commit_message>
Updating Outcomes.xlsx - SVR
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\Actual\Simulacion\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\Actual\Simulacion\Proyecto\ML_ParkinsonDisease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4915B0-DF72-4D19-8B62-47162623B20F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE66AC8A-33EA-4A05-8443-7402A6095783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MLR" sheetId="1" r:id="rId1"/>
     <sheet name="PW" sheetId="2" r:id="rId2"/>
     <sheet name="ANN" sheetId="3" r:id="rId3"/>
     <sheet name="RF" sheetId="4" r:id="rId4"/>
+    <sheet name="SVR" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="307">
   <si>
     <t>poly_degree</t>
   </si>
@@ -751,13 +752,211 @@
   </si>
   <si>
     <t>{'layers': (32, 32, 32), 'max_iter: 1500</t>
+  </si>
+  <si>
+    <t>{'C': 0.01, 'gamma': 0.01, 'kernel': 'linear'}</t>
+  </si>
+  <si>
+    <t>0.583880</t>
+  </si>
+  <si>
+    <t>-0.191601</t>
+  </si>
+  <si>
+    <t>0.233549</t>
+  </si>
+  <si>
+    <t>0.774820</t>
+  </si>
+  <si>
+    <t>{'C': 0.01, 'gamma': 0.01, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.739670</t>
+  </si>
+  <si>
+    <t>-0.153300</t>
+  </si>
+  <si>
+    <t>0.215761</t>
+  </si>
+  <si>
+    <t>0.782439</t>
+  </si>
+  <si>
+    <t>{'C': 0.01, 'gamma': 0.1, 'kernel': 'linear'}</t>
+  </si>
+  <si>
+    <t>{'C': 0.01, 'gamma': 0.1, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.682692</t>
+  </si>
+  <si>
+    <t>-0.156301</t>
+  </si>
+  <si>
+    <t>0.203188</t>
+  </si>
+  <si>
+    <t>0.745043</t>
+  </si>
+  <si>
+    <t>{'C': 0.01, 'gamma': 1, 'kernel': 'linear'}</t>
+  </si>
+  <si>
+    <t>{'C': 0.01, 'gamma': 1, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.718521</t>
+  </si>
+  <si>
+    <t>-0.152179</t>
+  </si>
+  <si>
+    <t>0.205011</t>
+  </si>
+  <si>
+    <t>0.755263</t>
+  </si>
+  <si>
+    <t>{'C': 1, 'gamma': 0.01, 'kernel': 'linear'}</t>
+  </si>
+  <si>
+    <t>0.467114</t>
+  </si>
+  <si>
+    <t>-0.354864</t>
+  </si>
+  <si>
+    <t>0.253703</t>
+  </si>
+  <si>
+    <t>0.705711</t>
+  </si>
+  <si>
+    <t>{'C': 1, 'gamma': 0.01, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.528497</t>
+  </si>
+  <si>
+    <t>-0.233535</t>
+  </si>
+  <si>
+    <t>0.221235</t>
+  </si>
+  <si>
+    <t>0.683757</t>
+  </si>
+  <si>
+    <t>{'C': 1, 'gamma': 0.1, 'kernel': 'linear'}</t>
+  </si>
+  <si>
+    <t>{'C': 1, 'gamma': 0.1, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.452823</t>
+  </si>
+  <si>
+    <t>-0.300730</t>
+  </si>
+  <si>
+    <t>0.207265</t>
+  </si>
+  <si>
+    <t>0.535530</t>
+  </si>
+  <si>
+    <t>{'C': 1, 'gamma': 1, 'kernel': 'linear'}</t>
+  </si>
+  <si>
+    <t>{'C': 1, 'gamma': 1, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.395171</t>
+  </si>
+  <si>
+    <t>-0.268098</t>
+  </si>
+  <si>
+    <t>0.149544</t>
+  </si>
+  <si>
+    <t>0.478966</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'gamma': 0.01, 'kernel': 'linear'}</t>
+  </si>
+  <si>
+    <t>0.477672</t>
+  </si>
+  <si>
+    <t>-0.372139</t>
+  </si>
+  <si>
+    <t>0.269904</t>
+  </si>
+  <si>
+    <t>0.753411</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'gamma': 0.01, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.449773</t>
+  </si>
+  <si>
+    <t>-0.306550</t>
+  </si>
+  <si>
+    <t>0.210868</t>
+  </si>
+  <si>
+    <t>0.535574</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'gamma': 0.1, 'kernel': 'linear'}</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'gamma': 0.1, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.522118</t>
+  </si>
+  <si>
+    <t>-0.414063</t>
+  </si>
+  <si>
+    <t>0.236925</t>
+  </si>
+  <si>
+    <t>0.570345</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'gamma': 1, 'kernel': 'linear'}</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'gamma': 1, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>0.398313</t>
+  </si>
+  <si>
+    <t>-0.402948</t>
+  </si>
+  <si>
+    <t>0.188868</t>
+  </si>
+  <si>
+    <t>0.469253</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -778,6 +977,19 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -815,7 +1027,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -840,6 +1052,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4902,7 +5126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6169,4 +6393,466 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D989DE4B-1122-4AED-B99F-6AB130C9511A}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="6.125" customWidth="1"/>
+    <col min="3" max="3" width="7.875" customWidth="1"/>
+    <col min="4" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="7.875" customWidth="1"/>
+    <col min="6" max="6" width="6.625" customWidth="1"/>
+    <col min="7" max="7" width="8.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="10">
+        <v>7223</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="10">
+        <v>8570</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" s="10">
+        <v>7168</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="F3" s="10">
+        <v>8441</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" s="10">
+        <v>7223</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4" s="10">
+        <v>8570</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="10">
+        <v>7201</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F5" s="10">
+        <v>8456</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" s="10">
+        <v>7223</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F6" s="10">
+        <v>8570</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="10">
+        <v>7160</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="F7" s="10">
+        <v>8440</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8" s="10">
+        <v>7487</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="10">
+        <v>9123</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B9" s="10">
+        <v>7327</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="F9" s="10">
+        <v>8718</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="B10" s="10">
+        <v>7487</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F10" s="10">
+        <v>9123</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11" s="10">
+        <v>7455</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="F11" s="10">
+        <v>8953</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="B12" s="10">
+        <v>7487</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F12" s="10">
+        <v>9123</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" s="10">
+        <v>7403</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="F13" s="10">
+        <v>8862</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="B14" s="10">
+        <v>7501</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F14" s="10">
+        <v>9177</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B15" s="10">
+        <v>7460</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="F15" s="10">
+        <v>8968</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B16" s="10">
+        <v>7501</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F16" s="10">
+        <v>9177</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B17" s="10">
+        <v>7747</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="F17" s="10">
+        <v>9330</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B18" s="10">
+        <v>7501</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F18" s="10">
+        <v>9177</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B19" s="10">
+        <v>7652</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="F19" s="10">
+        <v>9310</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>